<commit_message>
feat : attack button UI
</commit_message>
<xml_diff>
--- a/Assets/Docs/InfoDocument.xlsx
+++ b/Assets/Docs/InfoDocument.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNITY\Portfolio\UnityWork\Assets\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DDA494-F4F6-4033-8E85-A5CF7B8AF7FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20838249-9208-4E0A-B68B-E96E56C77610}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1860" windowWidth="14832" windowHeight="8964" activeTab="3" xr2:uid="{BB02A303-4D39-475C-93A2-B35DFE769B3C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BB02A303-4D39-475C-93A2-B35DFE769B3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>스킬ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,9 +64,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FireBallEffect</t>
-  </si>
-  <si>
     <t>회오리불꽃</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -103,34 +100,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>빨간도깨비</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>파란도깨비</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">보유스킬 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>10002/10102/10202</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>모델이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RedMonster</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BlueMonster</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>캐릭터 모델</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -167,7 +144,135 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>101/102</t>
+    <t>UI 이미지 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill_FireThrow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill_FireSpin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TinyFireEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BigFireEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잎날가르기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물대포</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BigGrassEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BigWaterEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill_GrassThrow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill_WaterThrow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초록이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빨강이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파랑이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10001/10101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flora</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fiery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cyclopes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10003/10103</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10002/10102</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TinyGrassEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TinyWaterEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모델 UI 이미지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model_Flora</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model_Fiery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model_Cyclopes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>104/105/106/107</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beezee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kaktos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ketchup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Woody</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쿨타임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BigFireEffect</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -535,7 +640,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -547,19 +652,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -567,16 +672,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C2">
-        <v>15000</v>
+        <v>5000</v>
       </c>
       <c r="D2">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
@@ -587,13 +692,13 @@
         <v>101</v>
       </c>
       <c r="C3">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="D3">
-        <v>270</v>
+        <v>400</v>
       </c>
       <c r="E3">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -601,16 +706,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C4">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="D4">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="E4">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -621,10 +726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD04E7C3-D286-4B42-93BB-29A63A362B13}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -632,11 +737,12 @@
     <col min="1" max="2" width="15.69921875" customWidth="1"/>
     <col min="3" max="3" width="20.19921875" customWidth="1"/>
     <col min="4" max="4" width="13.296875" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="16.3984375" customWidth="1"/>
+    <col min="5" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="16.3984375" customWidth="1"/>
+    <col min="8" max="8" width="14.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -644,24 +750,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -672,11 +784,14 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>10001</v>
       </c>
@@ -690,13 +805,16 @@
         <v>1</v>
       </c>
       <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>10002</v>
       </c>
@@ -710,13 +828,16 @@
         <v>1</v>
       </c>
       <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>10003</v>
       </c>
@@ -730,64 +851,132 @@
         <v>1</v>
       </c>
       <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>10102</v>
+        <v>10101</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7">
-        <v>10202</v>
+        <v>10102</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>1.5</v>
       </c>
       <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>10103</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>1.5</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>10202</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>1.7</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A788EE-46C3-4A0F-917F-2674C2F57274}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -795,49 +984,120 @@
     <col min="1" max="1" width="10.19921875" customWidth="1"/>
     <col min="2" max="2" width="12.69921875" customWidth="1"/>
     <col min="3" max="3" width="17.19921875" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="11.09765625" customWidth="1"/>
+    <col min="5" max="5" width="20.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>10003</v>
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="C5">
+        <v>10001</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="C6">
+        <v>10001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="C7">
+        <v>10001</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>107</v>
+      </c>
+      <c r="C8">
+        <v>10001</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -851,7 +1111,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -864,19 +1124,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -884,16 +1144,16 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>500</v>
       </c>
       <c r="D2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat : organize scene
</commit_message>
<xml_diff>
--- a/Assets/Docs/InfoDocument.xlsx
+++ b/Assets/Docs/InfoDocument.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNITY\Portfolio\UnityWork\Assets\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20838249-9208-4E0A-B68B-E96E56C77610}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3860A076-852B-49CA-9F68-C52F67BC364C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BB02A303-4D39-475C-93A2-B35DFE769B3C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BB02A303-4D39-475C-93A2-B35DFE769B3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>스킬ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -273,6 +273,10 @@
   </si>
   <si>
     <t>BigFireEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레벨</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -637,20 +641,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA95F9E-2D46-4102-9B81-4BF2A80B6E82}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="13.296875" customWidth="1"/>
-    <col min="2" max="2" width="12.796875" customWidth="1"/>
-    <col min="3" max="8" width="11.69921875" customWidth="1"/>
+    <col min="2" max="3" width="12.796875" customWidth="1"/>
+    <col min="4" max="9" width="11.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -658,16 +662,19 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -675,16 +682,19 @@
         <v>102</v>
       </c>
       <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
         <v>5000</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>500</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -692,16 +702,19 @@
         <v>101</v>
       </c>
       <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
         <v>3000</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>400</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -709,12 +722,15 @@
         <v>103</v>
       </c>
       <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
         <v>3000</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>450</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>60</v>
       </c>
     </row>
@@ -1110,7 +1126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF522975-A7EA-4246-B83E-C1A84893A44C}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>